<commit_message>
womp lots of reading in data
</commit_message>
<xml_diff>
--- a/cleanData/BookStores.xlsx
+++ b/cleanData/BookStores.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Desktop\Projects\School\DataVisProj\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicamurdock/Documents/GitHub/DataVisProj/cleanData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E158C2AE-C7E1-4FB5-9D9F-20BD12CEAB68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8EDB83D-8507-064C-8876-D445D0D2C3F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6195" yWindow="3420" windowWidth="21600" windowHeight="11385" xr2:uid="{97B2FBDD-39A2-4D54-93E4-C62CE2D2C5A5}"/>
+    <workbookView xWindow="4000" yWindow="3160" windowWidth="21600" windowHeight="11380" xr2:uid="{97B2FBDD-39A2-4D54-93E4-C62CE2D2C5A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>2011</t>
   </si>
@@ -91,6 +91,15 @@
   </si>
   <si>
     <t>Barnes and Noble</t>
+  </si>
+  <si>
+    <t>http://beta.barnesandnobleinc.com/documents/bn_annual_report_2010.pdf</t>
+  </si>
+  <si>
+    <t>https://slate.com/business/2014/09/independent-bookstores-rising-they-cant-compete-with-amazon-and-dont-have-to.html</t>
+  </si>
+  <si>
+    <t>https://www.hbs.edu/faculty/Publication%20Files/20-068_c19963e7-506c-479a-beb4-bb339cd293ee.pdf</t>
   </si>
 </sst>
 </file>
@@ -451,21 +460,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8458A4A-6C32-4E4D-A0C4-0ECC18A304FD}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="3" max="3" width="24.5" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -479,7 +488,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -492,8 +501,11 @@
       <c r="D2" s="3">
         <v>681</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -507,7 +519,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -521,7 +533,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
@@ -535,7 +547,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>2009</v>
       </c>
@@ -548,8 +560,11 @@
       <c r="D6" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -563,7 +578,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
@@ -577,7 +592,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -591,7 +606,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -605,7 +620,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
@@ -618,8 +633,11 @@
       <c r="D11" s="3">
         <v>661</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
@@ -633,7 +651,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>6</v>
       </c>
@@ -647,7 +665,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
@@ -661,7 +679,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
@@ -675,7 +693,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
@@ -689,7 +707,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2020</v>
       </c>

</xml_diff>